<commit_message>
Setting up final experimentation of real datasets
</commit_message>
<xml_diff>
--- a/experiments/actual_all_speedups/excel/EMS-GT-NPRIME2.xlsx
+++ b/experiments/actual_all_speedups/excel/EMS-GT-NPRIME2.xlsx
@@ -14,7 +14,7 @@
     <sheet name="15,5" sheetId="5" r:id="rId5"/>
     <sheet name="17,6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -924,7 +924,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1592,7 +1591,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2260,7 +2258,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2928,7 +2925,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3596,7 +3592,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4264,7 +4259,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>